<commit_message>
now print out volume used from each well after writing protocol
</commit_message>
<xml_diff>
--- a/inputs/211102_ECHO_source_plate_CRISPRtitration.xlsx
+++ b/inputs/211102_ECHO_source_plate_CRISPRtitration.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rycar\Documents\GitHub\WHISPR\inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4CF667D-D24D-416C-8099-5B9300F6B196}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC02F08B-0DDD-44C8-9BE5-FB8BB4D6DF95}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{546D7F41-76BF-4117-BD41-03A67E651BAB}"/>
   </bookViews>
@@ -693,7 +693,7 @@
   <dimension ref="A1:X33"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.83984375" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -765,7 +765,7 @@
         <v>511</v>
       </c>
       <c r="E3" s="3">
-        <v>50</v>
+        <v>24.2</v>
       </c>
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
@@ -801,7 +801,7 @@
         <v>223</v>
       </c>
       <c r="E4" s="3">
-        <v>50</v>
+        <v>31.6</v>
       </c>
       <c r="F4" s="1"/>
       <c r="G4" s="1"/>
@@ -837,7 +837,7 @@
         <v>115.5</v>
       </c>
       <c r="E5" s="3">
-        <v>50</v>
+        <v>65</v>
       </c>
       <c r="F5" s="1"/>
       <c r="G5" s="1"/>
@@ -873,7 +873,7 @@
         <v>157</v>
       </c>
       <c r="E6" s="3">
-        <v>50</v>
+        <v>33</v>
       </c>
       <c r="F6" s="1"/>
       <c r="G6" s="1"/>
@@ -909,7 +909,7 @@
         <v>116.6</v>
       </c>
       <c r="E7" s="3">
-        <v>50</v>
+        <v>65</v>
       </c>
       <c r="F7" s="1"/>
       <c r="G7" s="1"/>
@@ -945,7 +945,7 @@
         <v>135.69999999999999</v>
       </c>
       <c r="E8" s="3">
-        <v>50</v>
+        <v>60</v>
       </c>
       <c r="F8" s="1"/>
       <c r="G8" s="1"/>
@@ -981,7 +981,7 @@
         <v>190.3</v>
       </c>
       <c r="E9" s="3">
-        <v>50</v>
+        <v>60</v>
       </c>
       <c r="F9" s="1"/>
       <c r="G9" s="1"/>
@@ -1017,7 +1017,7 @@
         <v>189.3</v>
       </c>
       <c r="E10" s="3">
-        <v>50</v>
+        <v>60</v>
       </c>
       <c r="F10" s="1"/>
       <c r="G10" s="1"/>
@@ -1053,7 +1053,7 @@
         <v>40</v>
       </c>
       <c r="E11" s="3">
-        <v>50</v>
+        <v>60</v>
       </c>
       <c r="F11" s="1"/>
       <c r="G11" s="1"/>
@@ -1089,7 +1089,7 @@
         <v>188</v>
       </c>
       <c r="E12" s="3">
-        <v>50</v>
+        <v>65</v>
       </c>
       <c r="F12" s="1"/>
       <c r="G12" s="1"/>
@@ -1578,7 +1578,7 @@
   <dimension ref="A1:I32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="K4" sqref="K4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.9453125" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>

</xml_diff>